<commit_message>
add updates to files definitions
</commit_message>
<xml_diff>
--- a/mode/NewEngineLevelAllUnlocked/NewEngineFormulas.xlsx
+++ b/mode/NewEngineLevelAllUnlocked/NewEngineFormulas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="128">
   <si>
     <t>Truck Name</t>
   </si>
@@ -864,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H164"/>
+  <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="H154" sqref="H154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,11 +921,11 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="5">
-        <f>MIN(F20:F164)</f>
+        <f>MIN(F20:F168)</f>
         <v>3.1E-2</v>
       </c>
       <c r="D4" s="5">
-        <f>MAX(F20:F164)</f>
+        <f>MAX(F20:F168)</f>
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
@@ -3265,7 +3265,7 @@
         <v>0</v>
       </c>
       <c r="H131" s="14">
-        <f t="shared" ref="H131:H149" si="22">ROUND(((F131-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" ref="H131:H154" si="22">ROUND(((F131-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>0</v>
       </c>
     </row>
@@ -3277,7 +3277,7 @@
         <v>370</v>
       </c>
       <c r="F132" s="1">
-        <f t="shared" ref="F132:F149" si="23">($E$130+B132)*(IF(B132&lt;=$C$8,1,0)*$D$8+IF(AND(B132&gt;$C$8,B132&lt;=$C$9),1,0)*$D$9+IF(AND(B132&gt;$C$9,B132&lt;=$C$10),1,0)*$D$10+IF(AND(B132&gt;$C$10,B132&lt;=$C$11),1,0)*$D$11+IF(AND(B132&gt;$C$11,B132&lt;=$C$12),1,0)*$D$12+IF(AND(B132&gt;$C$12,B132&lt;=$C$13),1,0)*$D$13+IF(AND(B132&gt;$C$13,B132&lt;=$C$14),1,0)*$D$14+IF(AND(B132&gt;$C$14,B132&lt;=$C$15),1,0)*$D$15+IF(AND(B132&gt;$C$15,B132&lt;=$C$16),1,0)*$D$16+IF(AND(B132&gt;$C$16,B132&lt;=$C$17),1,0)*$D$17)</f>
+        <f t="shared" ref="F132:F154" si="23">($E$130+B132)*(IF(B132&lt;=$C$8,1,0)*$D$8+IF(AND(B132&gt;$C$8,B132&lt;=$C$9),1,0)*$D$9+IF(AND(B132&gt;$C$9,B132&lt;=$C$10),1,0)*$D$10+IF(AND(B132&gt;$C$10,B132&lt;=$C$11),1,0)*$D$11+IF(AND(B132&gt;$C$11,B132&lt;=$C$12),1,0)*$D$12+IF(AND(B132&gt;$C$12,B132&lt;=$C$13),1,0)*$D$13+IF(AND(B132&gt;$C$13,B132&lt;=$C$14),1,0)*$D$14+IF(AND(B132&gt;$C$14,B132&lt;=$C$15),1,0)*$D$15+IF(AND(B132&gt;$C$15,B132&lt;=$C$16),1,0)*$D$16+IF(AND(B132&gt;$C$16,B132&lt;=$C$17),1,0)*$D$17)</f>
         <v>3.7000000000000005E-2</v>
       </c>
       <c r="G132" s="1">
@@ -3626,268 +3626,347 @@
         <f>($F$2*C150)+($H$2*D150)</f>
         <v>0</v>
       </c>
-      <c r="H150" s="14"/>
+      <c r="H150" s="14">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="151" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B151" s="1">
-        <v>540</v>
+        <v>420</v>
       </c>
       <c r="F151" s="1">
-        <f>($E$150+B151)*(IF(B151&lt;=$C$8,1,0)*$D$8+IF(AND(B151&gt;$C$8,B151&lt;=$C$9),1,0)*$D$9+IF(AND(B151&gt;$C$9,B151&lt;=$C$10),1,0)*$D$10+IF(AND(B151&gt;$C$10,B151&lt;=$C$11),1,0)*$D$11+IF(AND(B151&gt;$C$11,B151&lt;=$C$12),1,0)*$D$12+IF(AND(B151&gt;$C$12,B151&lt;=$C$13),1,0)*$D$13+IF(AND(B151&gt;$C$13,B151&lt;=$C$14),1,0)*$D$14+IF(AND(B151&gt;$C$14,B151&lt;=$C$15),1,0)*$D$15+IF(AND(B151&gt;$C$15,B151&lt;=$C$16),1,0)*$D$16+IF(AND(B151&gt;$C$16,B151&lt;=$C$17),1,0)*$D$17)</f>
-        <v>5.3999999999999999E-2</v>
+        <f t="shared" si="23"/>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="G151" s="1">
         <v>0</v>
       </c>
       <c r="H151" s="14">
-        <f>ROUND(((F151-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B152" s="1">
-        <v>600</v>
+        <v>460</v>
       </c>
       <c r="F152" s="1">
-        <f>($E$150+B152)*(IF(B152&lt;=$C$8,1,0)*$D$8+IF(AND(B152&gt;$C$8,B152&lt;=$C$9),1,0)*$D$9+IF(AND(B152&gt;$C$9,B152&lt;=$C$10),1,0)*$D$10+IF(AND(B152&gt;$C$10,B152&lt;=$C$11),1,0)*$D$11+IF(AND(B152&gt;$C$11,B152&lt;=$C$12),1,0)*$D$12+IF(AND(B152&gt;$C$12,B152&lt;=$C$13),1,0)*$D$13+IF(AND(B152&gt;$C$13,B152&lt;=$C$14),1,0)*$D$14+IF(AND(B152&gt;$C$14,B152&lt;=$C$15),1,0)*$D$15+IF(AND(B152&gt;$C$15,B152&lt;=$C$16),1,0)*$D$16+IF(AND(B152&gt;$C$16,B152&lt;=$C$17),1,0)*$D$17)</f>
-        <v>6.0000000000000005E-2</v>
+        <f t="shared" si="23"/>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G152" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H152" s="14">
-        <f>ROUND(((F152-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B153" s="1">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="F153" s="1">
-        <f>($E$150+B153)*(IF(B153&lt;=$C$8,1,0)*$D$8+IF(AND(B153&gt;$C$8,B153&lt;=$C$9),1,0)*$D$9+IF(AND(B153&gt;$C$9,B153&lt;=$C$10),1,0)*$D$10+IF(AND(B153&gt;$C$10,B153&lt;=$C$11),1,0)*$D$11+IF(AND(B153&gt;$C$11,B153&lt;=$C$12),1,0)*$D$12+IF(AND(B153&gt;$C$12,B153&lt;=$C$13),1,0)*$D$13+IF(AND(B153&gt;$C$13,B153&lt;=$C$14),1,0)*$D$14+IF(AND(B153&gt;$C$14,B153&lt;=$C$15),1,0)*$D$15+IF(AND(B153&gt;$C$15,B153&lt;=$C$16),1,0)*$D$16+IF(AND(B153&gt;$C$16,B153&lt;=$C$17),1,0)*$D$17)</f>
-        <v>7.0000000000000007E-2</v>
+        <f t="shared" si="23"/>
+        <v>0.05</v>
       </c>
       <c r="G153" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H153" s="14">
-        <f>ROUND(((F153-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B154" s="1">
-        <v>750</v>
+        <v>540</v>
       </c>
       <c r="F154" s="1">
-        <f>($E$150+B154)*(IF(B154&lt;=$C$8,1,0)*$D$8+IF(AND(B154&gt;$C$8,B154&lt;=$C$9),1,0)*$D$9+IF(AND(B154&gt;$C$9,B154&lt;=$C$10),1,0)*$D$10+IF(AND(B154&gt;$C$10,B154&lt;=$C$11),1,0)*$D$11+IF(AND(B154&gt;$C$11,B154&lt;=$C$12),1,0)*$D$12+IF(AND(B154&gt;$C$12,B154&lt;=$C$13),1,0)*$D$13+IF(AND(B154&gt;$C$13,B154&lt;=$C$14),1,0)*$D$14+IF(AND(B154&gt;$C$14,B154&lt;=$C$15),1,0)*$D$15+IF(AND(B154&gt;$C$15,B154&lt;=$C$16),1,0)*$D$16+IF(AND(B154&gt;$C$16,B154&lt;=$C$17),1,0)*$D$17)</f>
-        <v>7.4999999999999997E-2</v>
+        <f t="shared" si="23"/>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="G154" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H154" s="14">
-        <f>ROUND(((F154-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A155" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B155" s="5"/>
-      <c r="C155" s="5">
-        <v>420</v>
-      </c>
-      <c r="D155" s="5">
-        <v>750</v>
-      </c>
-      <c r="E155" s="5">
-        <f>($F$2*C155)+($H$2*D155)</f>
-        <v>0</v>
-      </c>
-      <c r="H155" s="14"/>
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B155" s="1">
+        <v>540</v>
+      </c>
+      <c r="F155" s="1">
+        <f>($E$150+B155)*(IF(B155&lt;=$C$8,1,0)*$D$8+IF(AND(B155&gt;$C$8,B155&lt;=$C$9),1,0)*$D$9+IF(AND(B155&gt;$C$9,B155&lt;=$C$10),1,0)*$D$10+IF(AND(B155&gt;$C$10,B155&lt;=$C$11),1,0)*$D$11+IF(AND(B155&gt;$C$11,B155&lt;=$C$12),1,0)*$D$12+IF(AND(B155&gt;$C$12,B155&lt;=$C$13),1,0)*$D$13+IF(AND(B155&gt;$C$13,B155&lt;=$C$14),1,0)*$D$14+IF(AND(B155&gt;$C$14,B155&lt;=$C$15),1,0)*$D$15+IF(AND(B155&gt;$C$15,B155&lt;=$C$16),1,0)*$D$16+IF(AND(B155&gt;$C$16,B155&lt;=$C$17),1,0)*$D$17)</f>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G155" s="1">
+        <v>0</v>
+      </c>
+      <c r="H155" s="14">
+        <f>ROUND(((F155-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="156" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B156" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="F156" s="1">
-        <f>($E$155+B156)*(IF(B156&lt;=$C$8,1,0)*$D$8+IF(AND(B156&gt;$C$8,B156&lt;=$C$9),1,0)*$D$9+IF(AND(B156&gt;$C$9,B156&lt;=$C$10),1,0)*$D$10+IF(AND(B156&gt;$C$10,B156&lt;=$C$11),1,0)*$D$11+IF(AND(B156&gt;$C$11,B156&lt;=$C$12),1,0)*$D$12+IF(AND(B156&gt;$C$12,B156&lt;=$C$13),1,0)*$D$13+IF(AND(B156&gt;$C$13,B156&lt;=$C$14),1,0)*$D$14+IF(AND(B156&gt;$C$14,B156&lt;=$C$15),1,0)*$D$15+IF(AND(B156&gt;$C$15,B156&lt;=$C$16),1,0)*$D$16+IF(AND(B156&gt;$C$16,B156&lt;=$C$17),1,0)*$D$17)</f>
-        <v>4.2000000000000003E-2</v>
+        <f>($E$150+B156)*(IF(B156&lt;=$C$8,1,0)*$D$8+IF(AND(B156&gt;$C$8,B156&lt;=$C$9),1,0)*$D$9+IF(AND(B156&gt;$C$9,B156&lt;=$C$10),1,0)*$D$10+IF(AND(B156&gt;$C$10,B156&lt;=$C$11),1,0)*$D$11+IF(AND(B156&gt;$C$11,B156&lt;=$C$12),1,0)*$D$12+IF(AND(B156&gt;$C$12,B156&lt;=$C$13),1,0)*$D$13+IF(AND(B156&gt;$C$13,B156&lt;=$C$14),1,0)*$D$14+IF(AND(B156&gt;$C$14,B156&lt;=$C$15),1,0)*$D$15+IF(AND(B156&gt;$C$15,B156&lt;=$C$16),1,0)*$D$16+IF(AND(B156&gt;$C$16,B156&lt;=$C$17),1,0)*$D$17)</f>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="G156" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H156" s="14">
-        <f t="shared" ref="H156:H164" si="24">ROUND(((F156-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <f>ROUND(((F156-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B157" s="1">
-        <v>460</v>
+        <v>700</v>
       </c>
       <c r="F157" s="1">
-        <f t="shared" ref="F157:F164" si="25">($E$155+B157)*(IF(B157&lt;=$C$8,1,0)*$D$8+IF(AND(B157&gt;$C$8,B157&lt;=$C$9),1,0)*$D$9+IF(AND(B157&gt;$C$9,B157&lt;=$C$10),1,0)*$D$10+IF(AND(B157&gt;$C$10,B157&lt;=$C$11),1,0)*$D$11+IF(AND(B157&gt;$C$11,B157&lt;=$C$12),1,0)*$D$12+IF(AND(B157&gt;$C$12,B157&lt;=$C$13),1,0)*$D$13+IF(AND(B157&gt;$C$13,B157&lt;=$C$14),1,0)*$D$14+IF(AND(B157&gt;$C$14,B157&lt;=$C$15),1,0)*$D$15+IF(AND(B157&gt;$C$15,B157&lt;=$C$16),1,0)*$D$16+IF(AND(B157&gt;$C$16,B157&lt;=$C$17),1,0)*$D$17)</f>
-        <v>4.5999999999999999E-2</v>
+        <f>($E$150+B157)*(IF(B157&lt;=$C$8,1,0)*$D$8+IF(AND(B157&gt;$C$8,B157&lt;=$C$9),1,0)*$D$9+IF(AND(B157&gt;$C$9,B157&lt;=$C$10),1,0)*$D$10+IF(AND(B157&gt;$C$10,B157&lt;=$C$11),1,0)*$D$11+IF(AND(B157&gt;$C$11,B157&lt;=$C$12),1,0)*$D$12+IF(AND(B157&gt;$C$12,B157&lt;=$C$13),1,0)*$D$13+IF(AND(B157&gt;$C$13,B157&lt;=$C$14),1,0)*$D$14+IF(AND(B157&gt;$C$14,B157&lt;=$C$15),1,0)*$D$15+IF(AND(B157&gt;$C$15,B157&lt;=$C$16),1,0)*$D$16+IF(AND(B157&gt;$C$16,B157&lt;=$C$17),1,0)*$D$17)</f>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G157" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H157" s="14">
-        <f t="shared" si="24"/>
+        <f>ROUND(((F157-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
         <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B158" s="1">
+        <v>750</v>
+      </c>
+      <c r="F158" s="1">
+        <f>($E$150+B158)*(IF(B158&lt;=$C$8,1,0)*$D$8+IF(AND(B158&gt;$C$8,B158&lt;=$C$9),1,0)*$D$9+IF(AND(B158&gt;$C$9,B158&lt;=$C$10),1,0)*$D$10+IF(AND(B158&gt;$C$10,B158&lt;=$C$11),1,0)*$D$11+IF(AND(B158&gt;$C$11,B158&lt;=$C$12),1,0)*$D$12+IF(AND(B158&gt;$C$12,B158&lt;=$C$13),1,0)*$D$13+IF(AND(B158&gt;$C$13,B158&lt;=$C$14),1,0)*$D$14+IF(AND(B158&gt;$C$14,B158&lt;=$C$15),1,0)*$D$15+IF(AND(B158&gt;$C$15,B158&lt;=$C$16),1,0)*$D$16+IF(AND(B158&gt;$C$16,B158&lt;=$C$17),1,0)*$D$17)</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G158" s="1">
+        <v>16</v>
+      </c>
+      <c r="H158" s="14">
+        <f>ROUND(((F158-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B159" s="5"/>
+      <c r="C159" s="5">
+        <v>420</v>
+      </c>
+      <c r="D159" s="5">
+        <v>750</v>
+      </c>
+      <c r="E159" s="5">
+        <f>($F$2*C159)+($H$2*D159)</f>
+        <v>0</v>
+      </c>
+      <c r="H159" s="14"/>
+    </row>
+    <row r="160" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B160" s="1">
+        <v>420</v>
+      </c>
+      <c r="F160" s="1">
+        <f>($E$159+B160)*(IF(B160&lt;=$C$8,1,0)*$D$8+IF(AND(B160&gt;$C$8,B160&lt;=$C$9),1,0)*$D$9+IF(AND(B160&gt;$C$9,B160&lt;=$C$10),1,0)*$D$10+IF(AND(B160&gt;$C$10,B160&lt;=$C$11),1,0)*$D$11+IF(AND(B160&gt;$C$11,B160&lt;=$C$12),1,0)*$D$12+IF(AND(B160&gt;$C$12,B160&lt;=$C$13),1,0)*$D$13+IF(AND(B160&gt;$C$13,B160&lt;=$C$14),1,0)*$D$14+IF(AND(B160&gt;$C$14,B160&lt;=$C$15),1,0)*$D$15+IF(AND(B160&gt;$C$15,B160&lt;=$C$16),1,0)*$D$16+IF(AND(B160&gt;$C$16,B160&lt;=$C$17),1,0)*$D$17)</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="G160" s="1">
+        <v>0</v>
+      </c>
+      <c r="H160" s="14">
+        <f t="shared" ref="H160:H168" si="24">ROUND(((F160-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B161" s="1">
+        <v>460</v>
+      </c>
+      <c r="F161" s="1">
+        <f t="shared" ref="F161:F168" si="25">($E$159+B161)*(IF(B161&lt;=$C$8,1,0)*$D$8+IF(AND(B161&gt;$C$8,B161&lt;=$C$9),1,0)*$D$9+IF(AND(B161&gt;$C$9,B161&lt;=$C$10),1,0)*$D$10+IF(AND(B161&gt;$C$10,B161&lt;=$C$11),1,0)*$D$11+IF(AND(B161&gt;$C$11,B161&lt;=$C$12),1,0)*$D$12+IF(AND(B161&gt;$C$12,B161&lt;=$C$13),1,0)*$D$13+IF(AND(B161&gt;$C$13,B161&lt;=$C$14),1,0)*$D$14+IF(AND(B161&gt;$C$14,B161&lt;=$C$15),1,0)*$D$15+IF(AND(B161&gt;$C$15,B161&lt;=$C$16),1,0)*$D$16+IF(AND(B161&gt;$C$16,B161&lt;=$C$17),1,0)*$D$17)</f>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="G161" s="1">
+        <v>0</v>
+      </c>
+      <c r="H161" s="14">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B158" s="1">
+      <c r="B162" s="1">
         <v>460</v>
       </c>
-      <c r="F158" s="1">
+      <c r="F162" s="1">
         <f t="shared" si="25"/>
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="G158" s="1">
+      <c r="G162" s="1">
         <v>2</v>
       </c>
-      <c r="H158" s="14">
+      <c r="H162" s="14">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
+    <row r="163" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B163" s="1">
         <v>500</v>
       </c>
-      <c r="F159" s="1">
+      <c r="F163" s="1">
         <f t="shared" si="25"/>
         <v>0.05</v>
       </c>
-      <c r="G159" s="1">
+      <c r="G163" s="1">
         <v>6</v>
       </c>
-      <c r="H159" s="14">
+      <c r="H163" s="14">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
+    <row r="164" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B164" s="1">
         <v>540</v>
       </c>
-      <c r="F160" s="1">
+      <c r="F164" s="1">
         <f t="shared" si="25"/>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="G160" s="1">
+      <c r="G164" s="1">
         <v>6</v>
       </c>
-      <c r="H160" s="14">
+      <c r="H164" s="14">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
+    <row r="165" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B165" s="1">
         <v>540</v>
       </c>
-      <c r="F161" s="1">
+      <c r="F165" s="1">
         <f t="shared" si="25"/>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="G161" s="1">
+      <c r="G165" s="1">
         <v>11</v>
       </c>
-      <c r="H161" s="14">
+      <c r="H165" s="14">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
+    <row r="166" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B162" s="1">
+      <c r="B166" s="1">
         <v>600</v>
       </c>
-      <c r="F162" s="1">
+      <c r="F166" s="1">
         <f t="shared" si="25"/>
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="G162" s="1">
+      <c r="G166" s="1">
         <v>10</v>
       </c>
-      <c r="H162" s="14">
+      <c r="H166" s="14">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
+    <row r="167" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B163" s="1">
+      <c r="B167" s="1">
         <v>700</v>
       </c>
-      <c r="F163" s="1">
+      <c r="F167" s="1">
         <f t="shared" si="25"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G163" s="1">
+      <c r="G167" s="1">
         <v>16</v>
       </c>
-      <c r="H163" s="14">
+      <c r="H167" s="14">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
+    <row r="168" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B168" s="1">
         <v>750</v>
       </c>
-      <c r="F164" s="1">
+      <c r="F168" s="1">
         <f t="shared" si="25"/>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G164" s="1">
+      <c r="G168" s="1">
         <v>16</v>
       </c>
-      <c r="H164" s="14">
+      <c r="H168" s="14">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>

</xml_diff>